<commit_message>
4th commit with taking Screenshot of failed TestCases and Two negative Scenarios of Login Feature.
</commit_message>
<xml_diff>
--- a/testdata/ShlokAdmin.xlsx
+++ b/testdata/ShlokAdmin.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815" firstSheet="3" activeTab="6"/>
+    <workbookView windowWidth="19815" windowHeight="7815"/>
   </bookViews>
   <sheets>
-    <sheet name="DataManageRole" sheetId="1" r:id="rId1"/>
-    <sheet name="DataBranchName" sheetId="2" r:id="rId2"/>
-    <sheet name="Datalogin" sheetId="3" r:id="rId3"/>
+    <sheet name="Datalogin" sheetId="3" r:id="rId1"/>
+    <sheet name="DataManageRole" sheetId="1" r:id="rId2"/>
+    <sheet name="DataBranchName" sheetId="2" r:id="rId3"/>
     <sheet name="DataAccessRights" sheetId="4" r:id="rId4"/>
     <sheet name="DataSubAdminEmail" sheetId="5" r:id="rId5"/>
     <sheet name="DataSubAdminNameList" sheetId="6" r:id="rId6"/>
@@ -20,7 +20,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+  <si>
+    <t>Usename</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>superadmin@gmail.com</t>
+  </si>
+  <si>
+    <t>admin@123</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>min123</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>superadmingmail.com</t>
+  </si>
   <si>
     <t>Role Name</t>
   </si>
@@ -38,18 +62,6 @@
   </si>
   <si>
     <t>Pranaballava Public School</t>
-  </si>
-  <si>
-    <t>Usename</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>superadmin@gmail.com</t>
-  </si>
-  <si>
-    <t>admin@123</t>
   </si>
   <si>
     <t>Accesss</t>
@@ -186,10 +198,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -238,14 +250,112 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,110 +370,12 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -392,186 +404,186 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -679,7 +691,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -694,6 +706,21 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -701,15 +728,63 @@
     </border>
     <border>
       <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -739,6 +814,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -749,203 +839,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -964,12 +1006,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="7" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="7" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1290,6 +1336,75 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="24.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="12.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:3">
+      <c r="A4" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="superadmin@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="admin@123"/>
+    <hyperlink ref="A3" r:id="rId1" display="superadmin@gmail.com" tooltip="mailto:superadmin@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId2" display="admin@123"/>
+    <hyperlink ref="A4" r:id="rId1" display="superadmingmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1303,17 +1418,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="8" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="12" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="12" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:1">
@@ -1325,7 +1440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:A4"/>
@@ -1341,64 +1456,23 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="8" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="18" t="s">
-        <v>4</v>
+      <c r="A2" s="14" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="19" t="s">
-        <v>5</v>
+      <c r="A3" s="15" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:1">
       <c r="A4" s="13"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
-  <cols>
-    <col min="1" max="1" width="24.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="12.2857142857143" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" ht="15.75" spans="1:2">
-      <c r="A2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="superadmin@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="admin@123"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1420,17 +1494,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="12" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:1">
       <c r="A3" s="13" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1455,22 +1529,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="8" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="9" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:1">
       <c r="A4" s="10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1500,47 +1574,47 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="7" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -1557,7 +1631,7 @@
   <sheetPr/>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1573,22 +1647,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1596,19 +1670,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>32</v>
+      <c r="D2" s="24" t="s">
+        <v>36</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>33</v>
+        <v>3</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1616,19 +1690,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>34</v>
+      <c r="D3" s="24" t="s">
+        <v>38</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1636,19 +1710,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>36</v>
+      <c r="D4" s="24" t="s">
+        <v>40</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1656,19 +1730,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1676,19 +1750,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>46</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1696,19 +1770,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1716,19 +1790,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>52</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1736,19 +1810,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>55</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First Demo Commit (Date - 28-03-22)
</commit_message>
<xml_diff>
--- a/testdata/ShlokAdmin.xlsx
+++ b/testdata/ShlokAdmin.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
   <si>
     <t>Usename</t>
   </si>
@@ -145,64 +145,97 @@
     <t>image</t>
   </si>
   <si>
-    <t>7586541218</t>
+    <t>yann Reynolds</t>
+  </si>
+  <si>
+    <t>reynr839@gmail.com</t>
+  </si>
+  <si>
+    <t>9986541218</t>
   </si>
   <si>
     <t>D:\Shlok Docs\Teacher Details\Teacher\MzE5NzYuanBn.jpg</t>
   </si>
   <si>
-    <t>7586541219</t>
+    <t>tyan ricky</t>
+  </si>
+  <si>
+    <t>rr@gmail.com</t>
+  </si>
+  <si>
+    <t>9986541219</t>
   </si>
   <si>
     <t>D:\Shlok Docs\Teacher Details\Teacher\NTI3NzIuanBn.jpg</t>
   </si>
   <si>
-    <t>7586541220</t>
+    <t>Jhon Carrey</t>
+  </si>
+  <si>
+    <t>iphtrt2022@gmail.com</t>
+  </si>
+  <si>
+    <t>9986541220</t>
   </si>
   <si>
     <t>D:\Shlok Docs\Teacher Details\Teacher\NzA2NTIuanBn.jpg</t>
   </si>
   <si>
-    <t>hss@gmail.com</t>
-  </si>
-  <si>
-    <t>7586541221</t>
+    <t>Finland Wolfhard</t>
+  </si>
+  <si>
+    <t>hfi@gmail.com</t>
+  </si>
+  <si>
+    <t>9986541221</t>
   </si>
   <si>
     <t>D:\Shlok Docs\Teacher Details\Teacher\NzA3NjguanBn.jpg</t>
   </si>
   <si>
-    <t>srogen@gmail.com</t>
-  </si>
-  <si>
-    <t>7586541222</t>
+    <t>Sethi Rogen</t>
+  </si>
+  <si>
+    <t>srogent@gmail.com</t>
+  </si>
+  <si>
+    <t>9986541222</t>
   </si>
   <si>
     <t>D:\Shlok Docs\Teacher Details\Teacher\ODk2OTIuanBn.jpg</t>
   </si>
   <si>
-    <t>mperry@mail.com</t>
-  </si>
-  <si>
-    <t>7586541223</t>
+    <t>Mtthew Perry</t>
+  </si>
+  <si>
+    <t>mpery@mail.com</t>
+  </si>
+  <si>
+    <t>9986541223</t>
   </si>
   <si>
     <t>D:\Shlok Docs\Teacher Details\Teacher\ODU5MzAuanBn.jpg</t>
   </si>
   <si>
-    <t>kWu@mail.com</t>
-  </si>
-  <si>
-    <t>7586541224</t>
+    <t>Krisa Wu</t>
+  </si>
+  <si>
+    <t>kWuiu@mail.com</t>
+  </si>
+  <si>
+    <t>9986541224</t>
   </si>
   <si>
     <t>D:\Shlok Docs\Teacher Details\Teacher\XzAxNDUxMzIuanBn.jpg</t>
   </si>
   <si>
-    <t>Samell@mail.com</t>
-  </si>
-  <si>
-    <t>7586541225</t>
+    <t>tteph Amell</t>
+  </si>
+  <si>
+    <t>Stamell@mail.com</t>
+  </si>
+  <si>
+    <t>9986541225</t>
   </si>
   <si>
     <t>D:\Shlok Docs\Teacher Details\Teacher\XzAyNjU2NzYuanBn.jpg</t>
@@ -214,13 +247,37 @@
     <t>kartik#gmail.com</t>
   </si>
   <si>
-    <t>987654321</t>
+    <t>9986541226</t>
   </si>
   <si>
     <t>abc</t>
   </si>
   <si>
-    <t>D:\Shlok Docs\Teacher Details\Teacher\XzAyNjU3NzYuanBn.jpg</t>
+    <t>D:\Shlok Docs\Newsletter\curicullam.pdf</t>
+  </si>
+  <si>
+    <t>Varun</t>
+  </si>
+  <si>
+    <t>harikrisna@gmail.com</t>
+  </si>
+  <si>
+    <t>9986541227</t>
+  </si>
+  <si>
+    <t>zxy@123</t>
+  </si>
+  <si>
+    <t>Avinit</t>
+  </si>
+  <si>
+    <t>Avinit@gmail.com</t>
+  </si>
+  <si>
+    <t>9986541228</t>
+  </si>
+  <si>
+    <t>avi@gmai</t>
   </si>
 </sst>
 </file>
@@ -228,10 +285,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -258,7 +315,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -266,7 +323,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -279,8 +336,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,6 +348,60 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -302,63 +414,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -378,13 +436,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -434,13 +491,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,163 +665,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -791,7 +848,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -811,15 +868,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -831,6 +879,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -875,145 +932,145 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1024,15 +1081,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="7" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="7" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="7" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="7" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1043,10 +1100,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1675,10 +1732,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1716,19 +1773,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1736,19 +1793,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1756,19 +1813,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1776,19 +1833,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1796,19 +1853,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1816,19 +1873,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>53</v>
+        <v>61</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1836,19 +1893,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>56</v>
+        <v>65</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1856,19 +1913,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>59</v>
+        <v>69</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1876,36 +1933,71 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11">
+        <v>76</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2">
         <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="sambit839@gmail.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="surebotqa@gmail.com"/>
-    <hyperlink ref="C4" r:id="rId3" display="iphonep2022@gmail.com"/>
-    <hyperlink ref="C5" r:id="rId4" display="hss@gmail.com"/>
-    <hyperlink ref="C6" r:id="rId5" display="srogen@gmail.com"/>
-    <hyperlink ref="C7" r:id="rId6" display="mperry@mail.com"/>
-    <hyperlink ref="C8" r:id="rId7" display="kWu@mail.com"/>
-    <hyperlink ref="C9" r:id="rId8" display="Samell@mail.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="reynr839@gmail.com" tooltip="mailto:reynr839@gmail.com"/>
+    <hyperlink ref="C3" r:id="rId2" display="rr@gmail.com" tooltip="mailto:rr@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="iphtrt2022@gmail.com" tooltip="mailto:iphtrt2022@gmail.com"/>
+    <hyperlink ref="C5" r:id="rId4" display="hfi@gmail.com" tooltip="mailto:hfi@gmail.com"/>
+    <hyperlink ref="C6" r:id="rId5" display="srogent@gmail.com" tooltip="mailto:srogent@gmail.com"/>
+    <hyperlink ref="C7" r:id="rId6" display="mpery@mail.com" tooltip="mailto:mpery@mail.com"/>
+    <hyperlink ref="C8" r:id="rId7" display="kWuiu@mail.com" tooltip="mailto:kWuiu@mail.com"/>
+    <hyperlink ref="C9" r:id="rId8" display="Stamell@mail.com" tooltip="mailto:Stamell@mail.com"/>
     <hyperlink ref="E2" r:id="rId9" display="admin@123"/>
     <hyperlink ref="E3" r:id="rId9" display="admin@123"/>
     <hyperlink ref="E4" r:id="rId9" display="admin@123"/>
@@ -1914,6 +2006,10 @@
     <hyperlink ref="E7" r:id="rId9" display="admin@123"/>
     <hyperlink ref="E8" r:id="rId9" display="admin@123"/>
     <hyperlink ref="E9" r:id="rId9" display="admin@123"/>
+    <hyperlink ref="C11" r:id="rId10" display="harikrisna@gmail.com" tooltip="mailto:harikrisna@gmail.com"/>
+    <hyperlink ref="E11" r:id="rId11" display="zxy@123"/>
+    <hyperlink ref="C12" r:id="rId12" display="Avinit@gmail.com" tooltip="mailto:Avinit@gmail.com"/>
+    <hyperlink ref="E12" r:id="rId13" display="avi@gmai"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>